<commit_message>
updated charts in prep for report
</commit_message>
<xml_diff>
--- a/energy_vs_income.xlsx
+++ b/energy_vs_income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\Una\DataSkills\Projects\income_and_bills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BDA335-2F3A-463A-920E-CD9546A9B99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F0E1B3-E47A-4E0C-8D07-2A33EBE195D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_2c_AHC" sheetId="16" r:id="rId1"/>
@@ -109,7 +109,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId18"/>
+    <pivotCache cacheId="5" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2011,12 +2011,6 @@
   <dxfs count="32">
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2787,6 +2781,12 @@
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <family val="2"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4865,7 +4865,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> low income and weekly energy (both £)</a:t>
+                  <a:t> average income after housing costs and weekly energy (both £)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -6114,7 +6114,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> energy as % of net low income</a:t>
+                  <a:t> energy as % of (net low weekly income - housing costs)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -7558,7 +7558,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$S$3</c15:sqref>
@@ -7608,7 +7608,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$A$4:$B$17</c15:sqref>
@@ -7710,7 +7710,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$S$4:$S$17</c15:sqref>
@@ -7766,7 +7766,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000011-0A6A-42BF-8F8A-DD322CA91584}"/>
                   </c:ext>
@@ -7779,7 +7779,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$U$3</c15:sqref>
@@ -7826,7 +7826,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$A$4:$B$17</c15:sqref>
@@ -7928,7 +7928,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$U$4:$U$17</c15:sqref>
@@ -7984,7 +7984,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000013-0A6A-42BF-8F8A-DD322CA91584}"/>
                   </c:ext>
@@ -7997,7 +7997,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$R$3</c15:sqref>
@@ -8047,7 +8047,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$A$4:$B$17</c15:sqref>
@@ -8149,7 +8149,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$R$4:$R$17</c15:sqref>
@@ -8205,7 +8205,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-0A6A-42BF-8F8A-DD322CA91584}"/>
                   </c:ext>
@@ -8218,7 +8218,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$P$3</c15:sqref>
@@ -8268,7 +8268,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$A$4:$B$17</c15:sqref>
@@ -8370,7 +8370,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$P$4:$P$17</c15:sqref>
@@ -8380,7 +8380,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-0A6A-42BF-8F8A-DD322CA91584}"/>
                   </c:ext>
@@ -8393,7 +8393,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$X$3</c15:sqref>
@@ -8440,7 +8440,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$A$4:$B$17</c15:sqref>
@@ -8542,7 +8542,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$X$4:$X$17</c15:sqref>
@@ -8598,7 +8598,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000016-0A6A-42BF-8F8A-DD322CA91584}"/>
                   </c:ext>
@@ -8611,7 +8611,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$Z$3</c15:sqref>
@@ -8658,7 +8658,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$A$4:$B$17</c15:sqref>
@@ -8760,7 +8760,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>earnings_energy_comparison!$Z$4:$Z$17</c15:sqref>
@@ -8816,7 +8816,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000018-0A6A-42BF-8F8A-DD322CA91584}"/>
                   </c:ext>
@@ -15806,7 +15806,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EBB58D30-9A5B-4F42-8C29-143034167B4A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15828,7 +15828,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3CAB498E-325C-47A2-AEE1-3357DD287861}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18110,12 +18110,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.4536</cdr:x>
-      <cdr:y>0.12126</cdr:y>
+      <cdr:x>0.43618</cdr:x>
+      <cdr:y>0.11184</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.64892</cdr:x>
-      <cdr:y>0.23824</cdr:y>
+      <cdr:x>0.6315</cdr:x>
+      <cdr:y>0.22882</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -18130,8 +18130,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4221199" y="736888"/>
-          <a:ext cx="1817633" cy="710882"/>
+          <a:off x="4055587" y="678497"/>
+          <a:ext cx="1816059" cy="709682"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -18484,12 +18484,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.52644</cdr:x>
-      <cdr:y>0.69018</cdr:y>
+      <cdr:x>0.46322</cdr:x>
+      <cdr:y>0.71487</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.70326</cdr:x>
-      <cdr:y>0.79095</cdr:y>
+      <cdr:x>0.63402</cdr:x>
+      <cdr:y>0.80869</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -18504,8 +18504,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4899000" y="4194164"/>
-          <a:ext cx="1645474" cy="612374"/>
+          <a:off x="4308547" y="4340086"/>
+          <a:ext cx="1588669" cy="569565"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -18632,7 +18632,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>if energy usage was halved (by</a:t>
+            <a:t>if energy usage were halved (by</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" baseline="0"/>
@@ -18650,7 +18650,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6084979"/>
+    <xdr:ext cx="9304587" cy="6077107"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -21702,7 +21702,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable10" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="7" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable10" cacheId="5" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="7" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1" chartFormat="1">
   <location ref="A3:B28" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField compact="0" outline="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -21820,7 +21820,7 @@
     <dataField name="Average of weekly pay" fld="2" subtotal="average" baseField="1" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="31">
+    <format dxfId="30">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0" selected="0"/>
@@ -21852,44 +21852,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A78DEB72-0BCD-4E25-8C2E-8356CF5991E4}" name="Average_annual_domestic_gas_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_13600kWh_year_Great_Britain" displayName="Average_annual_domestic_gas_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_13600kWh_year_Great_Britain" ref="A13:M25" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" headerRowCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A78DEB72-0BCD-4E25-8C2E-8356CF5991E4}" name="Average_annual_domestic_gas_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_13600kWh_year_Great_Britain" displayName="Average_annual_domestic_gas_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_13600kWh_year_Great_Britain" ref="A13:M25" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowCellStyle="Normal">
   <autoFilter ref="A13:M25" xr:uid="{A78DEB72-0BCD-4E25-8C2E-8356CF5991E4}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{30BD38D5-17E1-4C20-AA72-65D57B5427CD}" name="Year" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{6B861553-9AF8-4D57-BD90-9E0B8321115F}" name="Standard credit: Home suppliers (pounds)" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{30BD38D5-17E1-4C20-AA72-65D57B5427CD}" name="Year" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{6B861553-9AF8-4D57-BD90-9E0B8321115F}" name="Standard credit: Home suppliers (pounds)" dataDxfId="26">
       <calculatedColumnFormula>ROUND([2]calc_new!C7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{34DC8BB4-DF60-4AB2-A9B8-B6E9A3CF3B51}" name="Standard credit: Non-home suppliers (pounds)" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{34DC8BB4-DF60-4AB2-A9B8-B6E9A3CF3B51}" name="Standard credit: Non-home suppliers (pounds)" dataDxfId="25">
       <calculatedColumnFormula>ROUND([2]calc_new!D7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{449F8710-B958-4F22-83EB-0437FC7BA359}" name="Standard credit: All consumers (pounds)" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{449F8710-B958-4F22-83EB-0437FC7BA359}" name="Standard credit: All consumers (pounds)" dataDxfId="24">
       <calculatedColumnFormula>ROUND([2]calc_new!E7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D0C86BCD-9F7C-4E55-AC46-58983E9726E1}" name="Direct debit: Home suppliers (pounds)" dataDxfId="24">
+    <tableColumn id="5" xr3:uid="{D0C86BCD-9F7C-4E55-AC46-58983E9726E1}" name="Direct debit: Home suppliers (pounds)" dataDxfId="23">
       <calculatedColumnFormula>ROUND([2]calc_new!G7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F0760AC4-3D2A-45FE-9139-E86D810327AB}" name="Direct debit: Non-home suppliers (pounds)" dataDxfId="23">
+    <tableColumn id="6" xr3:uid="{F0760AC4-3D2A-45FE-9139-E86D810327AB}" name="Direct debit: Non-home suppliers (pounds)" dataDxfId="22">
       <calculatedColumnFormula>ROUND([2]calc_new!H7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{741AC686-5706-4258-A29E-6EC199AE341D}" name="Direct debit: All consumers (pounds)" dataDxfId="22">
+    <tableColumn id="7" xr3:uid="{741AC686-5706-4258-A29E-6EC199AE341D}" name="Direct debit: All consumers (pounds)" dataDxfId="21">
       <calculatedColumnFormula>ROUND([2]calc_new!I7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{3E2B3AB2-EEFC-4398-9023-308A84997B1C}" name="Prepayment: Home suppliers (pounds)" dataDxfId="21">
+    <tableColumn id="8" xr3:uid="{3E2B3AB2-EEFC-4398-9023-308A84997B1C}" name="Prepayment: Home suppliers (pounds)" dataDxfId="20">
       <calculatedColumnFormula>ROUND([2]calc_new!K7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{ECFB11A5-2D9E-48BC-A2B1-4C76DDE1E0E0}" name="Prepayment: Non-home suppliers (pounds)" dataDxfId="20">
+    <tableColumn id="9" xr3:uid="{ECFB11A5-2D9E-48BC-A2B1-4C76DDE1E0E0}" name="Prepayment: Non-home suppliers (pounds)" dataDxfId="19">
       <calculatedColumnFormula>ROUND([2]calc_new!L7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C102352-1CDF-4D1E-BC72-77441FAE49FE}" name="Prepayment: All consumers (pounds)" dataDxfId="19">
+    <tableColumn id="10" xr3:uid="{0C102352-1CDF-4D1E-BC72-77441FAE49FE}" name="Prepayment: All consumers (pounds)" dataDxfId="18">
       <calculatedColumnFormula>ROUND([2]calc_new!M7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7521195B-BCD3-4B8D-A2C8-F77F6E45E8A3}" name="Overall: Home suppliers (pounds)" dataDxfId="18">
+    <tableColumn id="11" xr3:uid="{7521195B-BCD3-4B8D-A2C8-F77F6E45E8A3}" name="Overall: Home suppliers (pounds)" dataDxfId="17">
       <calculatedColumnFormula>ROUND([2]calc_new!O7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E20D2093-EAAD-43D8-9FBB-5CE39DD91F78}" name="Overall: Non-home suppliers (pounds)" dataDxfId="17">
+    <tableColumn id="12" xr3:uid="{E20D2093-EAAD-43D8-9FBB-5CE39DD91F78}" name="Overall: Non-home suppliers (pounds)" dataDxfId="16">
       <calculatedColumnFormula>ROUND([2]calc_new!P7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F40BE037-E6B6-41A5-A784-9D1BEC56253C}" name="Overall: UK (pounds)" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{F40BE037-E6B6-41A5-A784-9D1BEC56253C}" name="Overall: UK (pounds)" dataDxfId="15">
       <calculatedColumnFormula>ROUND([2]calc_new!Q7,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -21898,44 +21898,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{429E7A40-E504-4982-9061-ADA53938FB27}" name="Average_annual_domestic_Standard_Electricity_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_3600kWh_year_United_Kingdom" displayName="Average_annual_domestic_Standard_Electricity_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_3600kWh_year_United_Kingdom" ref="A9:M21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{429E7A40-E504-4982-9061-ADA53938FB27}" name="Average_annual_domestic_Standard_Electricity_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_3600kWh_year_United_Kingdom" displayName="Average_annual_domestic_Standard_Electricity_bills_in_cash_terms_by_home_and_non_home_supplier_based_on_consumption_of_3600kWh_year_United_Kingdom" ref="A9:M21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal">
   <autoFilter ref="A9:M21" xr:uid="{429E7A40-E504-4982-9061-ADA53938FB27}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A2263EB7-6357-4080-8F28-BDC9454EF550}" name="Year" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{BC21DD0A-3253-4497-888B-76D603023FF6}" name="Standard credit: Home suppliers (pounds)" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{A2263EB7-6357-4080-8F28-BDC9454EF550}" name="Year" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{BC21DD0A-3253-4497-888B-76D603023FF6}" name="Standard credit: Home suppliers (pounds)" dataDxfId="11">
       <calculatedColumnFormula>[3]calc_new!C7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8163651-9FFE-4A49-B3D4-8DD414CEB205}" name="Standard credit: Non-home suppliers (pounds)" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{B8163651-9FFE-4A49-B3D4-8DD414CEB205}" name="Standard credit: Non-home suppliers (pounds)" dataDxfId="10">
       <calculatedColumnFormula>[3]calc_new!D7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B183ABB5-9FB4-4016-9BFC-D80AF262841C}" name="Standard credit: All consumers (pounds)" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{B183ABB5-9FB4-4016-9BFC-D80AF262841C}" name="Standard credit: All consumers (pounds)" dataDxfId="9">
       <calculatedColumnFormula>[3]calc_new!E7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D44B4B46-27EE-4C16-8AAC-F2F92B0C2C90}" name="Direct debit: Home suppliers (pounds)" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{D44B4B46-27EE-4C16-8AAC-F2F92B0C2C90}" name="Direct debit: Home suppliers (pounds)" dataDxfId="8">
       <calculatedColumnFormula>[3]calc_new!F7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{32DE5A24-EC6F-45DB-BBAE-476670ED5B07}" name="Direct debit: Non-home suppliers (pounds)" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{32DE5A24-EC6F-45DB-BBAE-476670ED5B07}" name="Direct debit: Non-home suppliers (pounds)" dataDxfId="7">
       <calculatedColumnFormula>[3]calc_new!G7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2D53E424-0C7F-458E-98EF-A0436BAB8F7E}" name="Direct debit: All consumers (pounds)" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{2D53E424-0C7F-458E-98EF-A0436BAB8F7E}" name="Direct debit: All consumers (pounds)" dataDxfId="6">
       <calculatedColumnFormula>[3]calc_new!H7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{F6BAC252-3D85-4708-97AB-711BCDC6CFC7}" name="Prepayment: Home suppliers (pounds)" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{F6BAC252-3D85-4708-97AB-711BCDC6CFC7}" name="Prepayment: Home suppliers (pounds)" dataDxfId="5">
       <calculatedColumnFormula>[3]calc_new!I7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A67F95AE-8155-45E8-901C-A3A266C77F92}" name="Prepayment: Non-home suppliers (pounds)" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{A67F95AE-8155-45E8-901C-A3A266C77F92}" name="Prepayment: Non-home suppliers (pounds)" dataDxfId="4">
       <calculatedColumnFormula>[3]calc_new!J7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{AA7D8D03-847B-4CFC-9836-36BFCD66E337}" name="Prepayment: All consumers (pounds)" dataDxfId="4">
+    <tableColumn id="10" xr3:uid="{AA7D8D03-847B-4CFC-9836-36BFCD66E337}" name="Prepayment: All consumers (pounds)" dataDxfId="3">
       <calculatedColumnFormula>[3]calc_new!K7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D8F056FC-28A9-46CD-BA03-D8813EA0AA07}" name="Overall: Home suppliers (pounds)" dataDxfId="3">
+    <tableColumn id="11" xr3:uid="{D8F056FC-28A9-46CD-BA03-D8813EA0AA07}" name="Overall: Home suppliers (pounds)" dataDxfId="2">
       <calculatedColumnFormula>[3]calc_new!L7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{3F647466-D196-4F0B-8985-75A0F37521F3}" name="Overall: Non-home suppliers (pounds)" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{3F647466-D196-4F0B-8985-75A0F37521F3}" name="Overall: Non-home suppliers (pounds)" dataDxfId="1">
       <calculatedColumnFormula>[3]calc_new!M7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{90D18E8B-FFE3-4147-B575-FCE86CD58F50}" name="Overall: UK (pounds)" dataDxfId="1">
+    <tableColumn id="13" xr3:uid="{90D18E8B-FFE3-4147-B575-FCE86CD58F50}" name="Overall: UK (pounds)" dataDxfId="0">
       <calculatedColumnFormula>[3]calc_new!N7</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -23923,7 +23923,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AB4:AC116">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="notBetween">
       <formula>-0.15</formula>
       <formula>0.15</formula>
     </cfRule>
@@ -25246,7 +25246,7 @@
         <v>455</v>
       </c>
       <c r="Y14" s="133">
-        <f t="shared" ref="Y14:AA16" si="21">100*O14/X14</f>
+        <f t="shared" ref="Y14:Y16" si="21">100*O14/X14</f>
         <v>5.1971034825922739</v>
       </c>
       <c r="Z14" s="9">

</xml_diff>